<commit_message>
Changes in scripts according the Problem Statement
</commit_message>
<xml_diff>
--- a/Documents/EDevelopmentLog.xlsx
+++ b/Documents/EDevelopmentLog.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>DEVELOPMENT LOG</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>https://github.com/ELITA04/Recommender_system/blob/master/Scripts/saving.py</t>
+  </si>
+  <si>
+    <t>Fixed bugs in final script</t>
   </si>
 </sst>
 </file>
@@ -320,16 +323,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -337,12 +337,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -721,7 +722,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -731,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,17 +755,17 @@
   <sheetData>
     <row r="1" spans="2:13" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B1" s="2"/>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
       <c r="L1" s="11"/>
       <c r="M1" s="3"/>
     </row>
@@ -975,10 +976,10 @@
       <c r="E13" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="21">
         <v>43998</v>
       </c>
-      <c r="I13" s="21"/>
+      <c r="I13" s="20"/>
       <c r="J13" t="s">
         <v>25</v>
       </c>
@@ -994,19 +995,19 @@
       <c r="D14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="22" t="s">
         <v>20</v>
       </c>
       <c r="F14" s="19">
         <v>44021</v>
       </c>
-      <c r="G14" s="27" t="s">
+      <c r="G14" s="22" t="s">
         <v>20</v>
       </c>
       <c r="H14" s="19">
         <v>44027</v>
       </c>
-      <c r="I14" s="24" t="s">
+      <c r="I14" s="26" t="s">
         <v>21</v>
       </c>
       <c r="J14" s="1" t="s">
@@ -1024,19 +1025,19 @@
       <c r="D15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="22" t="s">
         <v>23</v>
       </c>
       <c r="F15" s="19">
         <v>44023</v>
       </c>
-      <c r="G15" s="27" t="s">
+      <c r="G15" s="22" t="s">
         <v>23</v>
       </c>
       <c r="H15" s="19">
         <v>44027</v>
       </c>
-      <c r="I15" s="24" t="s">
+      <c r="I15" s="26" t="s">
         <v>24</v>
       </c>
       <c r="J15" s="1" t="s">
@@ -1054,19 +1055,19 @@
       <c r="D16" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="27" t="s">
+      <c r="E16" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="F16" s="22">
+      <c r="F16" s="21">
         <v>44030</v>
       </c>
-      <c r="G16" s="27" t="s">
+      <c r="G16" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="22">
+      <c r="H16" s="21">
         <v>44032</v>
       </c>
-      <c r="I16" s="23" t="s">
+      <c r="I16" s="27" t="s">
         <v>31</v>
       </c>
       <c r="J16" t="s">
@@ -1084,17 +1085,19 @@
       <c r="D17" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="27" t="s">
+      <c r="E17" s="22" t="s">
         <v>27</v>
       </c>
       <c r="F17" s="19">
         <v>44027</v>
       </c>
-      <c r="G17" s="27" t="s">
+      <c r="G17" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="20" t="s">
+      <c r="H17" s="19">
+        <v>44033</v>
+      </c>
+      <c r="I17" s="23" t="s">
         <v>28</v>
       </c>
       <c r="J17" s="1" t="s">
@@ -1109,7 +1112,7 @@
       <c r="C18" s="1">
         <v>6</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="23" t="s">
         <v>34</v>
       </c>
       <c r="E18" s="18" t="s">
@@ -1118,9 +1121,15 @@
       <c r="F18" s="19">
         <v>44034</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
+      <c r="G18" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="19">
+        <v>44036</v>
+      </c>
+      <c r="I18" s="28" t="s">
+        <v>36</v>
+      </c>
       <c r="J18" s="1" t="s">
         <v>25</v>
       </c>
@@ -1759,12 +1768,13 @@
     <hyperlink ref="G14" r:id="rId8"/>
     <hyperlink ref="G17" r:id="rId9"/>
     <hyperlink ref="E18" r:id="rId10"/>
+    <hyperlink ref="G18" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
   <tableParts count="2">
-    <tablePart r:id="rId12"/>
     <tablePart r:id="rId13"/>
+    <tablePart r:id="rId14"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>